<commit_message>
modified to new header names
</commit_message>
<xml_diff>
--- a/tests/mixed_orders.xlsx
+++ b/tests/mixed_orders.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Insulin\Documents\Coding\Python Coding\cointracker-v2-git\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9995A70D-3345-45A6-8D3F-C5F64DBD9A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AEB988-0C55-480C-A9E6-1406E881B372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6924" yWindow="4824" windowWidth="34560" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10500" yWindow="4632" windowWidth="30192" windowHeight="16884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
   <si>
     <t>Date(UTC)</t>
   </si>
@@ -57,18 +57,6 @@
     <t>Fee</t>
   </si>
   <si>
-    <t>Fee Coin</t>
-  </si>
-  <si>
-    <t>Market 1 USD Spot Price</t>
-  </si>
-  <si>
-    <t>Market 2 USD Spot Price</t>
-  </si>
-  <si>
-    <t>Fee Coin USD Spot Price</t>
-  </si>
-  <si>
     <t>ETH-USD</t>
   </si>
   <si>
@@ -85,6 +73,18 @@
   </si>
   <si>
     <t>USD</t>
+  </si>
+  <si>
+    <t>Market 1 Fiat Spot Price</t>
+  </si>
+  <si>
+    <t>Market 2 Fiat Spot Price</t>
+  </si>
+  <si>
+    <t>Fee Asset Fiat Spot Price</t>
+  </si>
+  <si>
+    <t>Fee Asset</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -437,16 +437,16 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -454,10 +454,10 @@
         <v>44590</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>1000</v>
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="I2">
         <f>D2</f>
@@ -491,10 +491,10 @@
         <v>44591</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>1100</v>
@@ -509,8 +509,11 @@
       <c r="G3">
         <v>0</v>
       </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
       <c r="I3">
-        <f t="shared" ref="I3:J9" si="1">D3</f>
+        <f t="shared" ref="I3:I9" si="1">D3</f>
         <v>1100</v>
       </c>
       <c r="J3">
@@ -525,10 +528,10 @@
         <v>44592</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>0.5</v>
@@ -543,6 +546,9 @@
       <c r="G4">
         <v>0</v>
       </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
       <c r="I4">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -559,10 +565,10 @@
         <v>44592</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>0.6</v>
@@ -577,6 +583,9 @@
       <c r="G5">
         <v>0</v>
       </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
       <c r="I5">
         <f t="shared" si="1"/>
         <v>0.6</v>
@@ -593,10 +602,10 @@
         <v>44593</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>2000</v>
@@ -611,6 +620,9 @@
       <c r="G6">
         <v>0</v>
       </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
       <c r="I6">
         <f t="shared" si="1"/>
         <v>2000</v>
@@ -627,10 +639,10 @@
         <v>44595</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>2200</v>
@@ -645,6 +657,9 @@
       <c r="G7">
         <v>0</v>
       </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
       <c r="I7">
         <f t="shared" si="1"/>
         <v>2200</v>
@@ -661,10 +676,10 @@
         <v>44600</v>
       </c>
       <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
         <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
       </c>
       <c r="D8">
         <v>1000</v>
@@ -679,6 +694,9 @@
       <c r="G8">
         <v>0</v>
       </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
       <c r="I8">
         <f t="shared" si="1"/>
         <v>1000</v>
@@ -695,10 +713,10 @@
         <v>44621.666666666664</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>0.75</v>
@@ -712,6 +730,9 @@
       </c>
       <c r="G9">
         <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
       </c>
       <c r="I9">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
all transaction times are now at 0:00 UTC
</commit_message>
<xml_diff>
--- a/tests/mixed_orders.xlsx
+++ b/tests/mixed_orders.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Insulin\Documents\Coding\Python Coding\cointracker-v2-git\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AEB988-0C55-480C-A9E6-1406E881B372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26525530-FD8D-4DB9-9BB9-E10D04100A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10500" yWindow="4632" windowWidth="30192" windowHeight="16884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10248" yWindow="4560" windowWidth="30192" windowHeight="16884" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="21">
   <si>
     <t>Date(UTC)</t>
   </si>
@@ -85,6 +86,18 @@
   </si>
   <si>
     <t>Fee Asset</t>
+  </si>
+  <si>
+    <t>ETH Amount</t>
+  </si>
+  <si>
+    <t>ETH Value</t>
+  </si>
+  <si>
+    <t>ADA Amount</t>
+  </si>
+  <si>
+    <t>ADA Value</t>
   </si>
 </sst>
 </file>
@@ -405,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -710,7 +723,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>44621.666666666664</v>
+        <v>44621</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -747,6 +760,466 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9995880A-549D-41D7-B10D-C0EAD4B47472}">
+  <dimension ref="A1:X9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" t="s">
+        <v>18</v>
+      </c>
+      <c r="W1" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>44590</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <f>D2*E2</f>
+        <v>5000</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2">
+        <f>D2</f>
+        <v>1000</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <v>5000</v>
+      </c>
+      <c r="T2">
+        <v>5</v>
+      </c>
+      <c r="U2">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>44591</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>1100</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F9" si="0">D3*E3</f>
+        <v>5500</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I9" si="1">D3</f>
+        <v>1100</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>5</v>
+      </c>
+      <c r="O3">
+        <v>5500</v>
+      </c>
+      <c r="T3">
+        <v>10</v>
+      </c>
+      <c r="U3">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>44592</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+      <c r="E4">
+        <v>5000</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>5000</v>
+      </c>
+      <c r="R4">
+        <v>2500</v>
+      </c>
+      <c r="W4">
+        <v>5000</v>
+      </c>
+      <c r="X4">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>44592</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>0.6</v>
+      </c>
+      <c r="E5">
+        <v>10000</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>10000</v>
+      </c>
+      <c r="R5">
+        <v>6000</v>
+      </c>
+      <c r="W5">
+        <v>15000</v>
+      </c>
+      <c r="X5">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>2000</v>
+      </c>
+      <c r="E6">
+        <v>0.5</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0.5</v>
+      </c>
+      <c r="O6">
+        <v>1000</v>
+      </c>
+      <c r="Q6">
+        <v>1000</v>
+      </c>
+      <c r="T6">
+        <v>10.5</v>
+      </c>
+      <c r="W6">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>44595</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>2200</v>
+      </c>
+      <c r="E7">
+        <v>0.5</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>2200</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>10</v>
+      </c>
+      <c r="Q7">
+        <v>15200</v>
+      </c>
+      <c r="T7">
+        <v>10</v>
+      </c>
+      <c r="W7">
+        <v>15200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>44600</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>1000</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>4</v>
+      </c>
+      <c r="T8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>0.75</v>
+      </c>
+      <c r="E9">
+        <v>12500</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>9375</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>2700</v>
+      </c>
+      <c r="W9">
+        <v>2700</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>